<commit_message>
Added theta to Stability Finder Finished rotationalExternalPlotter Reset both spreadsheets to account for recording theta Added comment to reexamine Master() Added function minAOfTheta() which finds minimum a2 as a function of theta Added function autoRotator(), which finds minimum a2 at theta=0, then sees if stability changes with different thetas MinAOfTheta() needs to still be tested for angles=20 (working on it now) Added sample file for rotation result
</commit_message>
<xml_diff>
--- a/StabilityConditions.xlsx
+++ b/StabilityConditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkhoury/Documents/GitHub/AstroResearch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkhoury/Documents/Astroresearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B59BBE-3736-6A46-9A3F-3B87237C9090}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B6318-C250-BB4C-848B-52479892F385}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{23D46FAF-0C99-5346-913F-BE757C0E48C2}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{23D46FAF-0C99-5346-913F-BE757C0E48C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>m1</t>
   </si>
@@ -54,7 +54,10 @@
     <t>hParam</t>
   </si>
   <si>
-    <t>100P</t>
+    <t>Θ</t>
+  </si>
+  <si>
+    <t>1000P</t>
   </si>
 </sst>
 </file>
@@ -99,13 +102,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,16 +427,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC85775-338A-2C45-8142-D6E431C1659B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
@@ -452,28 +458,268 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>1.5</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>33.2802</v>
+        <v>13.51</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>0.01</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>13.69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0.01</v>
+      </c>
+      <c r="H3">
+        <v>180.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>13.97</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>13.88</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>0.01</v>
+      </c>
+      <c r="H5">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>13.26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>0.01</v>
+      </c>
+      <c r="H6">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>14.9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>0.01</v>
+      </c>
+      <c r="H7">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>14.52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>0.01</v>
+      </c>
+      <c r="H8">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>13.87</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>0.01</v>
+      </c>
+      <c r="H9">
+        <v>108.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>13.78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>0.01</v>
+      </c>
+      <c r="H10">
+        <v>126.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>13.97</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>0.01</v>
+      </c>
+      <c r="H11">
+        <v>144.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Formatting Issues in spreadsheets
</commit_message>
<xml_diff>
--- a/StabilityConditions.xlsx
+++ b/StabilityConditions.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>m1</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>1000P</t>
+  </si>
+  <si>
+    <t>10P</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC85775-338A-2C45-8142-D6E431C1659B}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -722,6 +725,396 @@
         <v>144.0</v>
       </c>
     </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>13.88</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>0.01</v>
+      </c>
+      <c r="H12">
+        <v>162.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>13.7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>0.01</v>
+      </c>
+      <c r="H13">
+        <v>198.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>13.89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>0.01</v>
+      </c>
+      <c r="H14">
+        <v>216.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>13.27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>0.01</v>
+      </c>
+      <c r="H15">
+        <v>234.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>14.91</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>0.01</v>
+      </c>
+      <c r="H16">
+        <v>252.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>15.41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>0.01</v>
+      </c>
+      <c r="H17">
+        <v>270.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>14.43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>0.01</v>
+      </c>
+      <c r="H18">
+        <v>288.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>13.78</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>0.01</v>
+      </c>
+      <c r="H19">
+        <v>306.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>13.97</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>0.01</v>
+      </c>
+      <c r="H20">
+        <v>324.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>14.4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>0.01</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>15.55</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <v>0.01</v>
+      </c>
+      <c r="H22">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>16.79</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>0.01</v>
+      </c>
+      <c r="H23">
+        <v>144.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>18.13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <v>0.01</v>
+      </c>
+      <c r="H24">
+        <v>216.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>14.32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <v>0.01</v>
+      </c>
+      <c r="H25">
+        <v>288.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>1.5</v>
+      </c>
+      <c r="B26">
+        <v>8.0</v>
+      </c>
+      <c r="C26">
+        <v>1.0</v>
+      </c>
+      <c r="D26">
+        <v>4.02</v>
+      </c>
+      <c r="E26">
+        <v>15.65</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>0.01</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>